<commit_message>
Added changes for: SetTransactionStatus, MaxConsecutiveExceptions, Add screenshot in transaction details for failed transactions.
</commit_message>
<xml_diff>
--- a/Reframework_update/VB/Data/Config.xlsx
+++ b/Reframework_update/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/UiPath/Reframework_update/VB/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{56E336E9-0DCF-4ADE-97BA-B11CA07F9DCD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -90,10 +90,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -122,6 +118,27 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveRetryNumber is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was exceeded. </t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>TestFramework</t>
   </si>
 </sst>
 </file>
@@ -497,18 +514,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -547,28 +564,36 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="43.2">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="28.8">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1561,6 +1586,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,16 +1596,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1616,7 +1644,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1624,79 +1652,96 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+    <row r="3" spans="1:26" ht="28.8">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
+      <c r="C11" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2672,6 +2717,7 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2682,16 +2728,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2702,7 +2746,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Moved Process.xaml to Framework folder. Added Retry for Get Transaction item. Added Retry for Set Transaction status.
</commit_message>
<xml_diff>
--- a/Reframework_update/VB/Data/Config.xlsx
+++ b/Reframework_update/VB/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/UiPath/Reframework_update/VB/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{56E336E9-0DCF-4ADE-97BA-B11CA07F9DCD}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{13386E9B-2A6C-42D9-AD45-2092F6427BAE}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>TestFramework</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
   </si>
 </sst>
 </file>
@@ -516,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1598,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1741,10 +1756,33 @@
       <c r="B12" t="s">
         <v>35</v>
       </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2728,7 +2766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>